<commit_message>
Updated mass remaining analysis script and added notes on analysis
</commit_message>
<xml_diff>
--- a/data/CompiledNecroDecomp_summer2017.xlsx
+++ b/data/CompiledNecroDecomp_summer2017.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10909"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11014"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Beidler/Shared/NecroDecomp_AMvsEMSettings/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{692CCD7B-40DC-9B48-A651-5B4EBE3727FF}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5CCC6B13-009F-6E41-8F06-FFC6EAC8B851}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="27320" windowHeight="13380" activeTab="1" xr2:uid="{AA2E3CDD-705C-A140-A963-890E0C23847C}"/>
   </bookViews>
@@ -33001,8 +33001,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{478EFE36-9A7C-CB4C-8073-D41103924A4C}">
   <dimension ref="A1:V488"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A20" sqref="A20:XFD20"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="S1" sqref="S1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -33066,7 +33066,7 @@
         <v>53</v>
       </c>
       <c r="S1" s="1" t="s">
-        <v>60</v>
+        <v>67</v>
       </c>
       <c r="T1" s="1" t="s">
         <v>59</v>
@@ -49900,7 +49900,7 @@
         <v>23.6</v>
       </c>
       <c r="Q247">
-        <f t="shared" ref="Q247:Q278" si="29">P247/100</f>
+        <f t="shared" ref="Q247:Q266" si="29">P247/100</f>
         <v>0.23600000000000002</v>
       </c>
       <c r="R247">
@@ -62867,7 +62867,7 @@
         <v>34.166666666666664</v>
       </c>
       <c r="Q435">
-        <f t="shared" ref="Q435:Q466" si="44">P435/100</f>
+        <f t="shared" ref="Q435:Q460" si="44">P435/100</f>
         <v>0.34166666666666662</v>
       </c>
       <c r="R435">
@@ -65157,7 +65157,7 @@
         <v>92</v>
       </c>
       <c r="S469">
-        <f t="shared" ref="S469:S532" si="47">R469/7</f>
+        <f t="shared" ref="S469:S488" si="47">R469/7</f>
         <v>13.142857142857142</v>
       </c>
       <c r="T469">

</xml_diff>